<commit_message>
Coding and configuring test environment
</commit_message>
<xml_diff>
--- a/ClientDemo/DataProvider/data.xlsx
+++ b/ClientDemo/DataProvider/data.xlsx
@@ -19,9 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>emma.hemmings@ampcusinc.com</t>
+  </si>
+  <si>
+    <t>Ginnie@123</t>
   </si>
 </sst>
 </file>
@@ -339,9 +342,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -349,9 +354,12 @@
     <col min="2" max="2" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
These are the recent changes
</commit_message>
<xml_diff>
--- a/ClientDemo/DataProvider/data.xlsx
+++ b/ClientDemo/DataProvider/data.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="3">
   <si>
     <t>emma.hemmings@ampcusinc.com</t>
   </si>
@@ -27,10 +27,7 @@
     <t>Ginnie@123</t>
   </si>
   <si>
-    <t>lhlhklhsdlkhlisdahlkisdhlskd</t>
-  </si>
-  <si>
-    <t>sjdjsdgdkljd</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -350,9 +347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -370,18 +365,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -389,7 +384,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>